<commit_message>
Fix framework from several issues
</commit_message>
<xml_diff>
--- a/data/SC_001_Google_Apps.xlsx
+++ b/data/SC_001_Google_Apps.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matheus.dias\Documents\IEWorkspace\Key\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matheusdias/Documents/git_repos/KeyFramework/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952223C8-F72F-487E-B8FB-974B5405D862}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2DED03E-32C6-1B48-98EC-A3CA177EFA3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{E31B522C-28CC-4738-9643-543934F79405}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20740" windowHeight="11160" xr2:uid="{E31B522C-28CC-4738-9643-543934F79405}"/>
   </bookViews>
   <sheets>
     <sheet name="TC_001_Google_Agenda" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
   <si>
     <t>vColuna4</t>
   </si>
@@ -53,6 +53,21 @@
   </si>
   <si>
     <t>vExpected Result</t>
+  </si>
+  <si>
+    <t>vGooglePassword</t>
+  </si>
+  <si>
+    <t>Zeca820@</t>
+  </si>
+  <si>
+    <t>Teste Executado com sucesso!</t>
+  </si>
+  <si>
+    <t>Coluna4</t>
+  </si>
+  <si>
+    <t>Coluna5</t>
   </si>
 </sst>
 </file>
@@ -136,7 +151,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
@@ -149,6 +164,7 @@
     <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -463,39 +479,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{596F6676-CC49-4EAC-B50F-ABE63B457FAA}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" customWidth="true" width="27.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="27.7109375" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="27.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="27.6640625" collapsed="true"/>
+    <col min="3" max="5" customWidth="true" width="27.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="2" t="s">
+      <c r="B2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -509,17 +536,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5124B344-A5E3-4F03-AC97-4CA88AE2CEFB}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" customWidth="true" width="27.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="27.7109375" collapsed="true"/>
+    <col min="1" max="4" customWidth="true" width="27.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -533,7 +559,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>

</xml_diff>